<commit_message>
Added description for the JavaDoc
</commit_message>
<xml_diff>
--- a/TANKS Documentation/Phase 3/Timeline.xlsx
+++ b/TANKS Documentation/Phase 3/Timeline.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Task to implement</t>
   </si>
@@ -96,6 +96,36 @@
   </si>
   <si>
     <t>Game does not crash</t>
+  </si>
+  <si>
+    <t>Planned Date</t>
+  </si>
+  <si>
+    <t>Pushed at the end due to optimization issued</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented earlier </t>
+  </si>
+  <si>
+    <t>Implementation of new elements</t>
+  </si>
+  <si>
+    <t>Testing on others</t>
+  </si>
+  <si>
+    <t>On time ~</t>
+  </si>
+  <si>
+    <t>Textures took longer to adjust</t>
+  </si>
+  <si>
+    <t>Had to wait for other implementations</t>
+  </si>
+  <si>
+    <t>Game mechanics had to be implemented</t>
+  </si>
+  <si>
+    <t>Added non-planned features (i.e. rotation)</t>
   </si>
 </sst>
 </file>
@@ -565,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:M14"/>
+  <dimension ref="E1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,9 +606,10 @@
     <col min="10" max="11" width="30.7109375" customWidth="1"/>
     <col min="12" max="12" width="33.85546875" customWidth="1"/>
     <col min="13" max="13" width="33.7109375" customWidth="1"/>
+    <col min="14" max="14" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
@@ -586,27 +617,33 @@
         <v>18</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="5:14" x14ac:dyDescent="0.25">
       <c r="J2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="6">
         <v>42792</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="6">
+        <v>42792</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E3" s="1"/>
       <c r="J3" s="9" t="s">
         <v>4</v>
@@ -614,146 +651,200 @@
       <c r="K3" s="10">
         <v>42831</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="10">
+        <v>42805</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="5:14" x14ac:dyDescent="0.25">
       <c r="J4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="10">
         <v>42815</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="10">
+        <v>42805</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:14" x14ac:dyDescent="0.25">
       <c r="J5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="K5" s="10">
         <v>42861</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="10">
+        <v>42812</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="5:14" x14ac:dyDescent="0.25">
       <c r="J6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="K6" s="10">
         <v>42817</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="10">
+        <v>42812</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="5:14" x14ac:dyDescent="0.25">
       <c r="J7" s="9" t="s">
         <v>8</v>
       </c>
       <c r="K7" s="10">
         <v>42831</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="10">
+        <v>42819</v>
+      </c>
+      <c r="M7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="5:14" x14ac:dyDescent="0.25">
       <c r="J8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K8" s="10">
         <v>42858</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="10">
+        <v>42829</v>
+      </c>
+      <c r="M8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="5:14" x14ac:dyDescent="0.25">
       <c r="J9" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K9" s="10">
         <v>42866</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="L9" s="10">
+        <v>42836</v>
+      </c>
+      <c r="M9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="7"/>
-    </row>
-    <row r="10" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="5:14" x14ac:dyDescent="0.25">
       <c r="J10" s="9" t="s">
         <v>11</v>
       </c>
       <c r="K10" s="10">
         <v>42865</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="10">
+        <v>42840</v>
+      </c>
+      <c r="M10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="7"/>
-    </row>
-    <row r="11" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="5:14" x14ac:dyDescent="0.25">
       <c r="J11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="K11" s="10">
         <v>42822</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="10">
+        <v>42849</v>
+      </c>
+      <c r="M11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="7"/>
-    </row>
-    <row r="12" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="5:14" x14ac:dyDescent="0.25">
       <c r="J12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K12" s="10">
         <v>42861</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="L12" s="10">
+        <v>42852</v>
+      </c>
+      <c r="M12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="7"/>
-    </row>
-    <row r="13" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="5:14" x14ac:dyDescent="0.25">
       <c r="J13" s="9" t="s">
         <v>14</v>
       </c>
       <c r="K13" s="10">
         <v>42861</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="L13" s="10">
+        <v>42855</v>
+      </c>
+      <c r="M13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="N13" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:14" x14ac:dyDescent="0.25">
       <c r="J14" s="9" t="s">
         <v>15</v>
       </c>
       <c r="K14" s="10">
         <v>42874</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="L14" s="10">
+        <v>42859</v>
+      </c>
+      <c r="M14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="N14" s="7" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>